<commit_message>
Correzione data.json e report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS/ARIANNAVACCINAZIONI/2303.05.01.00/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS/ARIANNAVACCINAZIONI/2303.05.01.00/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/davide_guidotti_dedalus_eu/Documents/FSE 2.0 Vaccinazioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="332" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4FDA534-0251-4706-9C00-F0AC84E27750}"/>
+  <xr:revisionPtr revIDLastSave="424" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FC8E3F6-ECC8-4661-BC48-992A461029A9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,78 +781,6 @@
     <t>Non è possibile da applicativo omettere il campo relativo alla data di somministrazione del vaccino</t>
   </si>
   <si>
-    <t>2023-03-30T15:23:26Z</t>
-  </si>
-  <si>
-    <t>92aca667fa0bc2a4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.4b530e9b0b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ef82f294c568181f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.93a509f6cd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-30T16:43:55Z</t>
-  </si>
-  <si>
-    <t>babf077db3db66e4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.7c8cf574d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-30T16:46:09Z</t>
-  </si>
-  <si>
-    <t>1dbd05fbf17b7563</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.7ce550209b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-30T16:48:07Z</t>
-  </si>
-  <si>
-    <t>1a1ed796cc3c43b0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.939f6285fb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-30T16:50:49Z</t>
-  </si>
-  <si>
-    <t>b77640c59a6893b7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.fe45f5ad81^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-30T16:59:19Z</t>
-  </si>
-  <si>
-    <t>d924c0d3d59ddaf4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.11b2cea753^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-30T17:00:51Z</t>
-  </si>
-  <si>
-    <t>618430b1f1d820fa</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.99283bc32c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-30T17:01:51Z</t>
-  </si>
-  <si>
     <t>subject_application_id:ARIANNAVACCINAZIONI</t>
   </si>
   <si>
@@ -871,145 +799,217 @@
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>8f6883a2a5b96991</t>
-  </si>
-  <si>
-    <t>1fbb1e4e7d82e70f</t>
-  </si>
-  <si>
-    <t>2023-03-31T11:09:28Z</t>
-  </si>
-  <si>
-    <t>2023-03-31T11:05:01Z</t>
-  </si>
-  <si>
-    <t>3cf106cf9e306061</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.039dc88df1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-31T11:20:38Z</t>
-  </si>
-  <si>
-    <t>529a6e34737556b4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.f22499570e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-31T11:26:42Z</t>
-  </si>
-  <si>
     <t>Viene segnalato un errore di timeout della validazione e si richiede all'utente di riprovare in un successivo momento</t>
   </si>
   <si>
-    <t>cb47d2b06ade0edf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.a6f11e8a79^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-31T15:24:40Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.8b543eb423^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>21950d2757362348</t>
-  </si>
-  <si>
-    <t>2023-03-31T15:51:41Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.3342b2c3a5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>afc925dfcd6c5af7</t>
-  </si>
-  <si>
-    <t>2023-03-31T15:59:40Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.305c56a64c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>83153eed6227689b</t>
-  </si>
-  <si>
-    <t>2023-03-31T16:02:25Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.8e3c65f3a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>b369a646de9e9e37</t>
-  </si>
-  <si>
-    <t>2023-03-31T16:12:15Z</t>
-  </si>
-  <si>
-    <t>ab7a39c846ce1854</t>
-  </si>
-  <si>
-    <t>2023-03-31T17:54:14Z</t>
-  </si>
-  <si>
-    <t>1160910120e4f2e1</t>
-  </si>
-  <si>
-    <t>2023-03-31T17:56:16Z</t>
-  </si>
-  <si>
-    <t>d4453069f194f42f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.eb3ffe5d5d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ba71fc891a465152</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.24cf816065^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-03T09:47:20Z</t>
-  </si>
-  <si>
-    <t>2023-04-03T09:44:59Z</t>
-  </si>
-  <si>
-    <t>9f91ac99b5e06f64</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.33960c7fa6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-03T09:48:28Z</t>
-  </si>
-  <si>
-    <t>6ce18f52ae423407</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.ba1759562a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-03T10:34:23Z</t>
-  </si>
-  <si>
-    <t>66b1cc85e535d1bb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.a6889d174e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-03T10:41:11Z</t>
-  </si>
-  <si>
     <t>Viene mostrato l'errore di ritorno dal gateway di validazione</t>
   </si>
   <si>
     <t>modifica dei dati non corretti e successivo reinvio</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:10:51Z</t>
+  </si>
+  <si>
+    <t>98e026e1626fb1ad</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.0ca71acfeb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>192c1df425864a09</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.186ff05850^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:12:31Z</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:13:21Z</t>
+  </si>
+  <si>
+    <t>3197c0b39422d07b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.8204c14d65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:15:29Z</t>
+  </si>
+  <si>
+    <t>8fef140246152c61</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.6e315525a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:28:50Z</t>
+  </si>
+  <si>
+    <t>6b312988bb585df1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.bb8c646e5d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:29:50Z</t>
+  </si>
+  <si>
+    <t>09dacbdbe9b77b25</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.073fc19079^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:30:34Z</t>
+  </si>
+  <si>
+    <t>0d8bf1a9ec51cd12</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.5d64d98182^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:31:16Z</t>
+  </si>
+  <si>
+    <t>26c94a70d6276d19</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.c1b34133f8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:23:12Z</t>
+  </si>
+  <si>
+    <t>43751b9d721ca397</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:27:35Z</t>
+  </si>
+  <si>
+    <t>b0151a4e921007c8</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:25:02Z</t>
+  </si>
+  <si>
+    <t>57394dc161066c5e</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:26:42Z</t>
+  </si>
+  <si>
+    <t>e5552155602826fb</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:18:15Z</t>
+  </si>
+  <si>
+    <t>f26b112fbb87ea71</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.d55fdce4ec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:19:13Z</t>
+  </si>
+  <si>
+    <t>1f3e19fe1e108bc6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.7d593d9564^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:20:07Z</t>
+  </si>
+  <si>
+    <t>7b73958a85d4a828</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.667dd966f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:20:56Z</t>
+  </si>
+  <si>
+    <t>f155c87c469f995f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.cc28ccf694^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:21:50Z</t>
+  </si>
+  <si>
+    <t>36eb187eb232b23d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.10e465b82a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:32:03Z</t>
+  </si>
+  <si>
+    <t>7844f06fde03ffa8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.66629f2bdf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:33:12Z</t>
+  </si>
+  <si>
+    <t>91afa793ef20b0e1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.7b9eb0315c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:34:06Z</t>
+  </si>
+  <si>
+    <t>b75fb102100fdf53</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.f2fcc4984e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:34:59Z</t>
+  </si>
+  <si>
+    <t>49c4e3ba24019b42</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.251d80ff67^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:35:52Z</t>
+  </si>
+  <si>
+    <t>f7fe1963b09edd6e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.a74a4c6c7d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:36:54Z</t>
+  </si>
+  <si>
+    <t>bd389b9b17e784ed</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.3619aadfed^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-06T09:37:43Z</t>
+  </si>
+  <si>
+    <t>62ad84821b8fcdcb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e58c93ad67fdab2a73460d24314be5a2f2227cb2a1d862863601f8fac621872.500cb832b9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1449,45 +1449,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3950,10 +3911,10 @@
   <dimension ref="A1:T669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="M27" sqref="M27"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4020,7 +3981,7 @@
       </c>
       <c r="B3" s="40"/>
       <c r="C3" s="45" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="D3" s="37"/>
       <c r="F3" s="12"/>
@@ -4043,7 +4004,7 @@
       <c r="A4" s="41"/>
       <c r="B4" s="42"/>
       <c r="C4" s="45" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="D4" s="37"/>
       <c r="E4" s="4"/>
@@ -4067,7 +4028,7 @@
       <c r="A5" s="43"/>
       <c r="B5" s="44"/>
       <c r="C5" s="45" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="D5" s="37"/>
       <c r="F5" s="12"/>
@@ -4222,16 +4183,16 @@
         <v>50</v>
       </c>
       <c r="F10" s="23">
-        <v>45015</v>
+        <v>45022</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>73</v>
@@ -4266,16 +4227,16 @@
         <v>52</v>
       </c>
       <c r="F11" s="23">
-        <v>45015</v>
+        <v>45022</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>73</v>
@@ -4310,16 +4271,16 @@
         <v>54</v>
       </c>
       <c r="F12" s="23">
-        <v>45015</v>
+        <v>45022</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>73</v>
@@ -4354,16 +4315,16 @@
         <v>56</v>
       </c>
       <c r="F13" s="23">
-        <v>45015</v>
+        <v>45022</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="H13" s="32" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="I13" s="32" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>73</v>
@@ -4398,16 +4359,16 @@
         <v>58</v>
       </c>
       <c r="F14" s="23">
-        <v>45015</v>
+        <v>45022</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>73</v>
@@ -4442,16 +4403,16 @@
         <v>60</v>
       </c>
       <c r="F15" s="23">
-        <v>45015</v>
+        <v>45022</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>73</v>
@@ -4486,16 +4447,16 @@
         <v>62</v>
       </c>
       <c r="F16" s="23">
-        <v>45015</v>
+        <v>45022</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="I16" s="32" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>73</v>
@@ -4530,16 +4491,16 @@
         <v>64</v>
       </c>
       <c r="F17" s="23">
-        <v>45015</v>
+        <v>45022</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="I17" s="32" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>73</v>
@@ -4574,16 +4535,16 @@
         <v>66</v>
       </c>
       <c r="F18" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>73</v>
@@ -4595,14 +4556,14 @@
       <c r="M18" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N18" s="58" t="s">
-        <v>223</v>
+      <c r="N18" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O18" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P18" s="58" t="s">
-        <v>224</v>
+      <c r="P18" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="26"/>
@@ -4628,16 +4589,16 @@
         <v>66</v>
       </c>
       <c r="F19" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>73</v>
@@ -4646,17 +4607,17 @@
       <c r="L19" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M19" s="58" t="s">
+      <c r="M19" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N19" s="58" t="s">
-        <v>223</v>
+      <c r="N19" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O19" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P19" s="58" t="s">
-        <v>224</v>
+      <c r="P19" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="26"/>
@@ -4682,16 +4643,16 @@
         <v>69</v>
       </c>
       <c r="F20" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>73</v>
@@ -4700,17 +4661,17 @@
       <c r="L20" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M20" s="58" t="s">
+      <c r="M20" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N20" s="58" t="s">
-        <v>223</v>
+      <c r="N20" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O20" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P20" s="58" t="s">
-        <v>224</v>
+      <c r="P20" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
@@ -4736,16 +4697,16 @@
         <v>71</v>
       </c>
       <c r="F21" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="H21" s="32" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>73</v>
@@ -4754,17 +4715,17 @@
       <c r="L21" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M21" s="58" t="s">
+      <c r="M21" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N21" s="58" t="s">
-        <v>223</v>
+      <c r="N21" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O21" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P21" s="58" t="s">
-        <v>224</v>
+      <c r="P21" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
@@ -4800,7 +4761,7 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="33" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="26" t="s">
@@ -4838,7 +4799,7 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="33" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="Q23" s="25"/>
       <c r="R23" s="26" t="s">
@@ -4980,35 +4941,35 @@
         <v>83</v>
       </c>
       <c r="F27" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="J27" s="33" t="s">
         <v>73</v>
       </c>
       <c r="K27" s="25"/>
-      <c r="L27" s="58" t="s">
+      <c r="L27" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M27" s="58" t="s">
+      <c r="M27" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N27" s="46" t="s">
-        <v>223</v>
+      <c r="N27" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O27" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P27" s="58" t="s">
-        <v>224</v>
+      <c r="P27" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
@@ -5041,7 +5002,7 @@
         <v>141</v>
       </c>
       <c r="K28" s="25" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="L28" s="25"/>
       <c r="M28" s="25"/>
@@ -5117,7 +5078,7 @@
         <v>141</v>
       </c>
       <c r="K30" s="25" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
@@ -5186,16 +5147,16 @@
         <v>93</v>
       </c>
       <c r="F32" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="H32" s="24" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="I32" s="24" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="J32" s="33" t="s">
         <v>73</v>
@@ -5204,17 +5165,17 @@
       <c r="L32" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M32" s="58" t="s">
+      <c r="M32" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N32" s="47" t="s">
-        <v>223</v>
+      <c r="N32" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O32" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P32" s="58" t="s">
-        <v>224</v>
+      <c r="P32" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="26"/>
@@ -5240,35 +5201,35 @@
         <v>95</v>
       </c>
       <c r="F33" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="J33" s="33" t="s">
         <v>73</v>
       </c>
       <c r="K33" s="25"/>
-      <c r="L33" s="58" t="s">
+      <c r="L33" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M33" s="58" t="s">
+      <c r="M33" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N33" s="48" t="s">
-        <v>223</v>
+      <c r="N33" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O33" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P33" s="58" t="s">
-        <v>224</v>
+      <c r="P33" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q33" s="25"/>
       <c r="R33" s="26"/>
@@ -5294,35 +5255,35 @@
         <v>97</v>
       </c>
       <c r="F34" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="H34" s="24" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="I34" s="24" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>73</v>
       </c>
       <c r="K34" s="25"/>
-      <c r="L34" s="58" t="s">
+      <c r="L34" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M34" s="58" t="s">
+      <c r="M34" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N34" s="49" t="s">
-        <v>223</v>
+      <c r="N34" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O34" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P34" s="58" t="s">
-        <v>224</v>
+      <c r="P34" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="26"/>
@@ -5386,35 +5347,35 @@
         <v>101</v>
       </c>
       <c r="F36" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="H36" s="24" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="I36" s="24" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="J36" s="33" t="s">
         <v>73</v>
       </c>
       <c r="K36" s="24"/>
-      <c r="L36" s="58" t="s">
+      <c r="L36" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M36" s="58" t="s">
+      <c r="M36" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N36" s="50" t="s">
-        <v>223</v>
+      <c r="N36" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O36" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P36" s="58" t="s">
-        <v>224</v>
+      <c r="P36" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q36" s="25"/>
       <c r="R36" s="26"/>
@@ -5554,35 +5515,35 @@
         <v>109</v>
       </c>
       <c r="F40" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G40" s="32" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="H40" s="32" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>183</v>
+        <v>206</v>
       </c>
       <c r="J40" s="33" t="s">
         <v>73</v>
       </c>
       <c r="K40" s="25"/>
-      <c r="L40" s="58" t="s">
+      <c r="L40" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M40" s="58" t="s">
+      <c r="M40" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N40" s="51" t="s">
-        <v>223</v>
+      <c r="N40" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O40" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P40" s="58" t="s">
-        <v>224</v>
+      <c r="P40" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q40" s="25"/>
       <c r="R40" s="26"/>
@@ -5615,7 +5576,7 @@
         <v>141</v>
       </c>
       <c r="K41" s="24" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="L41" s="25"/>
       <c r="M41" s="25"/>
@@ -5691,7 +5652,7 @@
         <v>141</v>
       </c>
       <c r="K43" s="25" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="L43" s="25"/>
       <c r="M43" s="25"/>
@@ -5722,35 +5683,35 @@
         <v>117</v>
       </c>
       <c r="F44" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G44" s="32" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="J44" s="33" t="s">
         <v>73</v>
       </c>
       <c r="K44" s="25"/>
-      <c r="L44" s="58" t="s">
+      <c r="L44" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M44" s="58" t="s">
+      <c r="M44" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N44" s="52" t="s">
-        <v>223</v>
+      <c r="N44" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O44" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P44" s="58" t="s">
-        <v>224</v>
+      <c r="P44" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q44" s="25"/>
       <c r="R44" s="26"/>
@@ -5814,35 +5775,35 @@
         <v>121</v>
       </c>
       <c r="F46" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="H46" s="32" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="I46" s="32" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="J46" s="33" t="s">
         <v>73</v>
       </c>
       <c r="K46" s="25"/>
-      <c r="L46" s="58" t="s">
+      <c r="L46" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M46" s="58" t="s">
+      <c r="M46" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N46" s="53" t="s">
-        <v>223</v>
+      <c r="N46" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O46" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P46" s="58" t="s">
-        <v>224</v>
+      <c r="P46" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="26"/>
@@ -5868,35 +5829,35 @@
         <v>123</v>
       </c>
       <c r="F47" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>192</v>
+        <v>215</v>
       </c>
       <c r="J47" s="33" t="s">
         <v>73</v>
       </c>
       <c r="K47" s="25"/>
-      <c r="L47" s="58" t="s">
+      <c r="L47" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M47" s="58" t="s">
+      <c r="M47" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N47" s="54" t="s">
-        <v>223</v>
+      <c r="N47" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O47" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P47" s="58" t="s">
-        <v>224</v>
+      <c r="P47" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
@@ -5922,35 +5883,35 @@
         <v>125</v>
       </c>
       <c r="F48" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="H48" s="24" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="I48" s="24" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
       <c r="J48" s="33" t="s">
         <v>73</v>
       </c>
       <c r="K48" s="25"/>
-      <c r="L48" s="58" t="s">
+      <c r="L48" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M48" s="58" t="s">
+      <c r="M48" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N48" s="55" t="s">
-        <v>223</v>
+      <c r="N48" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O48" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P48" s="58" t="s">
-        <v>224</v>
+      <c r="P48" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q48" s="25"/>
       <c r="R48" s="26"/>
@@ -6014,35 +5975,35 @@
         <v>129</v>
       </c>
       <c r="F50" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="H50" s="24" t="s">
-        <v>199</v>
+        <v>220</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="J50" s="33" t="s">
         <v>73</v>
       </c>
       <c r="K50" s="25"/>
-      <c r="L50" s="58" t="s">
+      <c r="L50" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M50" s="58" t="s">
+      <c r="M50" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N50" s="56" t="s">
-        <v>223</v>
+      <c r="N50" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O50" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P50" s="58" t="s">
-        <v>224</v>
+      <c r="P50" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q50" s="25"/>
       <c r="R50" s="26"/>
@@ -6068,35 +6029,35 @@
         <v>131</v>
       </c>
       <c r="F51" s="23">
-        <v>45016</v>
+        <v>45022</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
       <c r="J51" s="33" t="s">
         <v>73</v>
       </c>
       <c r="K51" s="25"/>
-      <c r="L51" s="58" t="s">
+      <c r="L51" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M51" s="58" t="s">
+      <c r="M51" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="N51" s="57" t="s">
-        <v>223</v>
+      <c r="N51" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="O51" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P51" s="58" t="s">
-        <v>224</v>
+      <c r="P51" s="25" t="s">
+        <v>156</v>
       </c>
       <c r="Q51" s="25"/>
       <c r="R51" s="26"/>

</xml_diff>

<commit_message>
Nuovo upload caso 16 AriannaVaccinazioni
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS/ARIANNAVACCINAZIONI/2303.05.01.00/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS/ARIANNAVACCINAZIONI/2303.05.01.00/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/davide_guidotti_dedalus_eu/Documents/FSE 2.0 Vaccinazioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="542" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E29BFF10-0480-4E86-97CD-C7E3188D4902}"/>
+  <xr:revisionPtr revIDLastSave="547" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8353A966-C433-4D31-9335-6698AAF04C29}"/>
   <bookViews>
-    <workbookView xWindow="23808" yWindow="768" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -973,15 +973,6 @@
     <t>2023-04-21T14:19:47Z</t>
   </si>
   <si>
-    <t>2023-04-21T14:18:36Z</t>
-  </si>
-  <si>
-    <t>019a065a72818639</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.b2174ac7ad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.9aa41de8bf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -1010,6 +1001,15 @@
   </si>
   <si>
     <t>2023-04-21T14:35:52Z</t>
+  </si>
+  <si>
+    <t>2023-05-04T10:36:25Z</t>
+  </si>
+  <si>
+    <t>f078434d28820e91</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.b0a1dd3697^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1754,10 +1754,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="130.109375" customWidth="1"/>
-    <col min="2" max="26" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="130.140625" customWidth="1"/>
+    <col min="2" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14.25" customHeight="1">
@@ -2818,11 +2818,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="2" width="194.109375" customWidth="1"/>
-    <col min="3" max="26" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="194.140625" customWidth="1"/>
+    <col min="3" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -2894,7 +2894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="43.2">
+    <row r="11" spans="1:2" ht="45">
       <c r="A11" s="10">
         <v>8</v>
       </c>
@@ -3914,27 +3914,27 @@
   <dimension ref="A1:T669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="D49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="46.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="63.88671875" customWidth="1"/>
-    <col min="5" max="5" width="104.88671875" customWidth="1"/>
-    <col min="6" max="9" width="33.109375" customWidth="1"/>
-    <col min="10" max="10" width="27.109375" customWidth="1"/>
-    <col min="11" max="15" width="36.44140625" customWidth="1"/>
-    <col min="16" max="16" width="27.109375" customWidth="1"/>
-    <col min="17" max="17" width="33.109375" customWidth="1"/>
-    <col min="18" max="18" width="36.44140625" customWidth="1"/>
-    <col min="19" max="20" width="31.88671875" customWidth="1"/>
-    <col min="21" max="26" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="63.85546875" customWidth="1"/>
+    <col min="5" max="5" width="104.85546875" customWidth="1"/>
+    <col min="6" max="9" width="33.140625" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" customWidth="1"/>
+    <col min="11" max="15" width="36.42578125" customWidth="1"/>
+    <col min="16" max="16" width="27.140625" customWidth="1"/>
+    <col min="17" max="17" width="33.140625" customWidth="1"/>
+    <col min="18" max="18" width="36.42578125" customWidth="1"/>
+    <col min="19" max="20" width="31.85546875" customWidth="1"/>
+    <col min="21" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.25" customHeight="1">
@@ -4169,7 +4169,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="129.6">
+    <row r="10" spans="1:20" ht="135">
       <c r="A10" s="20">
         <v>16</v>
       </c>
@@ -4186,16 +4186,16 @@
         <v>50</v>
       </c>
       <c r="F10" s="23">
-        <v>45037</v>
+        <v>45050</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>73</v>
@@ -4213,7 +4213,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="129.6">
+    <row r="11" spans="1:20" ht="135">
       <c r="A11" s="20">
         <v>17</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="12" spans="1:20" ht="135.75" thickBot="1">
       <c r="A12" s="20">
         <v>18</v>
       </c>
@@ -4280,10 +4280,10 @@
         <v>211</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>73</v>
@@ -4301,7 +4301,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="13" spans="1:20" ht="135.75" thickBot="1">
       <c r="A13" s="20">
         <v>19</v>
       </c>
@@ -4324,10 +4324,10 @@
         <v>210</v>
       </c>
       <c r="H13" s="32" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I13" s="32" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>73</v>
@@ -4345,7 +4345,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="14" spans="1:20" ht="150.75" thickBot="1">
       <c r="A14" s="20">
         <v>20</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="15" spans="1:20" ht="150.75" thickBot="1">
       <c r="A15" s="20">
         <v>21</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="16" spans="1:20" ht="150.75" thickBot="1">
       <c r="A16" s="20">
         <v>22</v>
       </c>
@@ -4453,13 +4453,13 @@
         <v>45037</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="I16" s="32" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>73</v>
@@ -4477,7 +4477,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="17" spans="1:20" ht="150.75" thickBot="1">
       <c r="A17" s="20">
         <v>23</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="18" spans="1:20" ht="150.75" thickBot="1">
       <c r="A18" s="20">
         <v>33</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="19" spans="1:20" ht="150.75" thickBot="1">
       <c r="A19" s="20">
         <v>34</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="144.6" thickBot="1">
+    <row r="20" spans="1:20" ht="165.75" thickBot="1">
       <c r="A20" s="20">
         <v>41</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="144.6" thickBot="1">
+    <row r="21" spans="1:20" ht="165.75" thickBot="1">
       <c r="A21" s="20">
         <v>42</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="58.2" thickBot="1">
+    <row r="22" spans="1:20" ht="75.75" thickBot="1">
       <c r="A22" s="20">
         <v>49</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="58.2" thickBot="1">
+    <row r="23" spans="1:20" ht="75.75" thickBot="1">
       <c r="A23" s="20">
         <v>50</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="129.6">
+    <row r="24" spans="1:20" ht="135">
       <c r="A24" s="20">
         <v>94</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="129.6">
+    <row r="25" spans="1:20" ht="135">
       <c r="A25" s="20">
         <v>95</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="101.4" thickBot="1">
+    <row r="26" spans="1:20" ht="105.75" thickBot="1">
       <c r="A26" s="20">
         <v>96</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="115.8" thickBot="1">
+    <row r="27" spans="1:20" ht="120.75" thickBot="1">
       <c r="A27" s="20">
         <v>97</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="28" spans="1:20" ht="135.75" thickBot="1">
       <c r="A28" s="20">
         <v>98</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="29" spans="1:20" ht="135.75" thickBot="1">
       <c r="A29" s="20">
         <v>99</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="100.8">
+    <row r="30" spans="1:20" ht="105">
       <c r="A30" s="20">
         <v>100</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="115.8" thickBot="1">
+    <row r="31" spans="1:20" ht="120.75" thickBot="1">
       <c r="A31" s="20">
         <v>101</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="32" spans="1:20" ht="135.75" thickBot="1">
       <c r="A32" s="20">
         <v>102</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="33" spans="1:20" ht="135.75" thickBot="1">
       <c r="A33" s="20">
         <v>103</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="101.4" thickBot="1">
+    <row r="34" spans="1:20" ht="105.75" thickBot="1">
       <c r="A34" s="20">
         <v>104</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="35" spans="1:20" ht="135.75" thickBot="1">
       <c r="A35" s="20">
         <v>105</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="36" spans="1:20" ht="135.75" thickBot="1">
       <c r="A36" s="20">
         <v>106</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="115.8" thickBot="1">
+    <row r="37" spans="1:20" ht="120.75" thickBot="1">
       <c r="A37" s="20">
         <v>107</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="115.8" thickBot="1">
+    <row r="38" spans="1:20" ht="120.75" thickBot="1">
       <c r="A38" s="20">
         <v>108</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="115.8" thickBot="1">
+    <row r="39" spans="1:20" ht="120.75" thickBot="1">
       <c r="A39" s="20">
         <v>109</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="101.4" thickBot="1">
+    <row r="40" spans="1:20" ht="105.75" thickBot="1">
       <c r="A40" s="20">
         <v>110</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="115.8" thickBot="1">
+    <row r="41" spans="1:20" ht="120.75" thickBot="1">
       <c r="A41" s="20">
         <v>111</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="115.8" thickBot="1">
+    <row r="42" spans="1:20" ht="120.75" thickBot="1">
       <c r="A42" s="20">
         <v>112</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="115.8" thickBot="1">
+    <row r="43" spans="1:20" ht="120.75" thickBot="1">
       <c r="A43" s="20">
         <v>113</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="115.8" thickBot="1">
+    <row r="44" spans="1:20" ht="120.75" thickBot="1">
       <c r="A44" s="20">
         <v>114</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="115.8" thickBot="1">
+    <row r="45" spans="1:20" ht="120.75" thickBot="1">
       <c r="A45" s="20">
         <v>115</v>
       </c>
@@ -5761,7 +5761,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="115.8" thickBot="1">
+    <row r="46" spans="1:20" ht="120.75" thickBot="1">
       <c r="A46" s="20">
         <v>116</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="115.8" thickBot="1">
+    <row r="47" spans="1:20" ht="120.75" thickBot="1">
       <c r="A47" s="20">
         <v>117</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="115.8" thickBot="1">
+    <row r="48" spans="1:20" ht="120.75" thickBot="1">
       <c r="A48" s="20">
         <v>118</v>
       </c>
@@ -5923,7 +5923,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="115.8" thickBot="1">
+    <row r="49" spans="1:20" ht="120.75" thickBot="1">
       <c r="A49" s="20">
         <v>119</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="115.8" thickBot="1">
+    <row r="50" spans="1:20" ht="120.75" thickBot="1">
       <c r="A50" s="20">
         <v>120</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="115.2">
+    <row r="51" spans="1:20" ht="120">
       <c r="A51" s="20">
         <v>121</v>
       </c>
@@ -6035,13 +6035,13 @@
         <v>45037</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J51" s="33" t="s">
         <v>73</v>
@@ -15713,15 +15713,15 @@
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="102" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
-    <col min="8" max="26" width="8.88671875" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1">
@@ -16725,11 +16725,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="26" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Correzione caso 16 AriannaVaccinazioni
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS/ARIANNAVACCINAZIONI/2303.05.01.00/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS/ARIANNAVACCINAZIONI/2303.05.01.00/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/davide_guidotti_dedalus_eu/Documents/FSE 2.0 Vaccinazioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="547" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8353A966-C433-4D31-9335-6698AAF04C29}"/>
+  <xr:revisionPtr revIDLastSave="555" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{576B52C8-7F76-4DE2-AFD5-A59BEC8B5DA5}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -1003,13 +1003,13 @@
     <t>2023-04-21T14:35:52Z</t>
   </si>
   <si>
-    <t>2023-05-04T10:36:25Z</t>
-  </si>
-  <si>
-    <t>f078434d28820e91</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.b0a1dd3697^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.167f83f2a44afefb8307a9b579ee4d10ee1ade2eab21684e92cb7f43a2589374.4bb7c9233a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5f31f2479a805df5</t>
+  </si>
+  <si>
+    <t>2023-05-15T17:54:16Z</t>
   </si>
 </sst>
 </file>
@@ -3917,7 +3917,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4186,16 +4186,16 @@
         <v>50</v>
       </c>
       <c r="F10" s="23">
-        <v>45050</v>
+        <v>45061</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="H10" s="32" t="s">
         <v>223</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
Aggiornamento checklist per casi 49 e 50
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS/ARIANNAVACCINAZIONI/2303.05.01.00/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS/ARIANNAVACCINAZIONI/2303.05.01.00/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/davide_guidotti_dedalus_eu/Documents/FSE 2.0 Vaccinazioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="555" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{576B52C8-7F76-4DE2-AFD5-A59BEC8B5DA5}"/>
+  <xr:revisionPtr revIDLastSave="560" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AA80D34-F263-4E36-A774-3B2B299BE726}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -799,9 +799,6 @@
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>Viene segnalato un errore di timeout della validazione e si richiede all'utente di riprovare in un successivo momento</t>
-  </si>
-  <si>
     <t>Viene mostrato l'errore di ritorno dal gateway di validazione</t>
   </si>
   <si>
@@ -1010,6 +1007,11 @@
   </si>
   <si>
     <t>2023-05-15T17:54:16Z</t>
+  </si>
+  <si>
+    <t>Viene segnalato un errore di timeout della validazione, il programma riproverà ad eseguire la validazione dopo un certo periodo di tempo (configurabile).
+Verranno eseguiti un certo numero di tentativi (anch'esso configurabile).
+In caso tutti i tentativi automatici falliscano, il record rimarrà marcato come in errore su database e verrà gestito da back office</t>
   </si>
 </sst>
 </file>
@@ -1754,10 +1756,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="130.140625" customWidth="1"/>
-    <col min="2" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="130.109375" customWidth="1"/>
+    <col min="2" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14.25" customHeight="1">
@@ -2818,11 +2820,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="194.140625" customWidth="1"/>
-    <col min="3" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="194.109375" customWidth="1"/>
+    <col min="3" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -2894,7 +2896,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="45">
+    <row r="11" spans="1:2" ht="43.2">
       <c r="A11" s="10">
         <v>8</v>
       </c>
@@ -3914,27 +3916,27 @@
   <dimension ref="A1:T669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="H20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" customWidth="1"/>
-    <col min="5" max="5" width="104.85546875" customWidth="1"/>
-    <col min="6" max="9" width="33.140625" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="15" width="36.42578125" customWidth="1"/>
-    <col min="16" max="16" width="27.140625" customWidth="1"/>
-    <col min="17" max="17" width="33.140625" customWidth="1"/>
-    <col min="18" max="18" width="36.42578125" customWidth="1"/>
-    <col min="19" max="20" width="31.85546875" customWidth="1"/>
-    <col min="21" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="46.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="63.88671875" customWidth="1"/>
+    <col min="5" max="5" width="104.88671875" customWidth="1"/>
+    <col min="6" max="9" width="33.109375" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" customWidth="1"/>
+    <col min="11" max="15" width="36.44140625" customWidth="1"/>
+    <col min="16" max="16" width="27.109375" customWidth="1"/>
+    <col min="17" max="17" width="33.109375" customWidth="1"/>
+    <col min="18" max="18" width="36.44140625" customWidth="1"/>
+    <col min="19" max="20" width="31.88671875" customWidth="1"/>
+    <col min="21" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.25" customHeight="1">
@@ -4169,7 +4171,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="135">
+    <row r="10" spans="1:20" ht="129.6">
       <c r="A10" s="20">
         <v>16</v>
       </c>
@@ -4189,13 +4191,13 @@
         <v>45061</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>73</v>
@@ -4213,7 +4215,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="135">
+    <row r="11" spans="1:20" ht="129.6">
       <c r="A11" s="20">
         <v>17</v>
       </c>
@@ -4233,13 +4235,13 @@
         <v>45029</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H11" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="I11" s="32" t="s">
         <v>165</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>166</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>73</v>
@@ -4257,7 +4259,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="135.75" thickBot="1">
+    <row r="12" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A12" s="20">
         <v>18</v>
       </c>
@@ -4277,13 +4279,13 @@
         <v>45037</v>
       </c>
       <c r="G12" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="I12" s="32" t="s">
         <v>211</v>
-      </c>
-      <c r="H12" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="I12" s="32" t="s">
-        <v>212</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>73</v>
@@ -4301,7 +4303,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="135.75" thickBot="1">
+    <row r="13" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A13" s="20">
         <v>19</v>
       </c>
@@ -4321,13 +4323,13 @@
         <v>45037</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H13" s="32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I13" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>73</v>
@@ -4345,7 +4347,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="150.75" thickBot="1">
+    <row r="14" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A14" s="20">
         <v>20</v>
       </c>
@@ -4365,13 +4367,13 @@
         <v>45029</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>73</v>
@@ -4389,7 +4391,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="150.75" thickBot="1">
+    <row r="15" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A15" s="20">
         <v>21</v>
       </c>
@@ -4409,13 +4411,13 @@
         <v>45029</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>73</v>
@@ -4433,7 +4435,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="150.75" thickBot="1">
+    <row r="16" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A16" s="20">
         <v>22</v>
       </c>
@@ -4453,13 +4455,13 @@
         <v>45037</v>
       </c>
       <c r="G16" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="H16" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="I16" s="32" t="s">
         <v>217</v>
-      </c>
-      <c r="I16" s="32" t="s">
-        <v>218</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>73</v>
@@ -4477,7 +4479,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="150.75" thickBot="1">
+    <row r="17" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A17" s="20">
         <v>23</v>
       </c>
@@ -4497,13 +4499,13 @@
         <v>45029</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I17" s="32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>73</v>
@@ -4521,7 +4523,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="150.75" thickBot="1">
+    <row r="18" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A18" s="20">
         <v>33</v>
       </c>
@@ -4541,10 +4543,10 @@
         <v>45022</v>
       </c>
       <c r="G18" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H18" s="24" t="s">
         <v>157</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>158</v>
       </c>
       <c r="I18" s="24" t="s">
         <v>153</v>
@@ -4560,13 +4562,13 @@
         <v>73</v>
       </c>
       <c r="N18" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O18" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P18" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="26"/>
@@ -4575,7 +4577,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="150.75" thickBot="1">
+    <row r="19" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A19" s="20">
         <v>34</v>
       </c>
@@ -4595,10 +4597,10 @@
         <v>45022</v>
       </c>
       <c r="G19" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" s="24" t="s">
         <v>159</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>160</v>
       </c>
       <c r="I19" s="24" t="s">
         <v>153</v>
@@ -4614,13 +4616,13 @@
         <v>73</v>
       </c>
       <c r="N19" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O19" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P19" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="26"/>
@@ -4629,7 +4631,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="165.75" thickBot="1">
+    <row r="20" spans="1:20" ht="144.6" thickBot="1">
       <c r="A20" s="20">
         <v>41</v>
       </c>
@@ -4649,10 +4651,10 @@
         <v>45022</v>
       </c>
       <c r="G20" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="H20" s="24" t="s">
         <v>161</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>162</v>
       </c>
       <c r="I20" s="24" t="s">
         <v>153</v>
@@ -4668,13 +4670,13 @@
         <v>73</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O20" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P20" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
@@ -4683,7 +4685,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="165.75" thickBot="1">
+    <row r="21" spans="1:20" ht="144.6" thickBot="1">
       <c r="A21" s="20">
         <v>42</v>
       </c>
@@ -4703,10 +4705,10 @@
         <v>45022</v>
       </c>
       <c r="G21" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="H21" s="32" t="s">
         <v>163</v>
-      </c>
-      <c r="H21" s="32" t="s">
-        <v>164</v>
       </c>
       <c r="I21" s="24" t="s">
         <v>153</v>
@@ -4722,13 +4724,13 @@
         <v>73</v>
       </c>
       <c r="N21" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O21" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P21" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
@@ -4737,7 +4739,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="75.75" thickBot="1">
+    <row r="22" spans="1:20" ht="202.2" thickBot="1">
       <c r="A22" s="20">
         <v>49</v>
       </c>
@@ -4764,7 +4766,7 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="33" t="s">
-        <v>154</v>
+        <v>224</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="26" t="s">
@@ -4775,7 +4777,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="75.75" thickBot="1">
+    <row r="23" spans="1:20" ht="202.2" thickBot="1">
       <c r="A23" s="20">
         <v>50</v>
       </c>
@@ -4802,7 +4804,7 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="33" t="s">
-        <v>154</v>
+        <v>224</v>
       </c>
       <c r="Q23" s="25"/>
       <c r="R23" s="26" t="s">
@@ -4813,7 +4815,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="135">
+    <row r="24" spans="1:20" ht="129.6">
       <c r="A24" s="20">
         <v>94</v>
       </c>
@@ -4851,7 +4853,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="135">
+    <row r="25" spans="1:20" ht="129.6">
       <c r="A25" s="20">
         <v>95</v>
       </c>
@@ -4889,7 +4891,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="105.75" thickBot="1">
+    <row r="26" spans="1:20" ht="101.4" thickBot="1">
       <c r="A26" s="20">
         <v>96</v>
       </c>
@@ -4927,7 +4929,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="120.75" thickBot="1">
+    <row r="27" spans="1:20" ht="115.8" thickBot="1">
       <c r="A27" s="20">
         <v>97</v>
       </c>
@@ -4947,13 +4949,13 @@
         <v>45029</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J27" s="33" t="s">
         <v>73</v>
@@ -4966,13 +4968,13 @@
         <v>73</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O27" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P27" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
@@ -4981,7 +4983,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="135.75" thickBot="1">
+    <row r="28" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A28" s="20">
         <v>98</v>
       </c>
@@ -5019,7 +5021,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="135.75" thickBot="1">
+    <row r="29" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A29" s="20">
         <v>99</v>
       </c>
@@ -5057,7 +5059,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="105">
+    <row r="30" spans="1:20" ht="100.8">
       <c r="A30" s="20">
         <v>100</v>
       </c>
@@ -5095,7 +5097,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="120.75" thickBot="1">
+    <row r="31" spans="1:20" ht="115.8" thickBot="1">
       <c r="A31" s="20">
         <v>101</v>
       </c>
@@ -5133,7 +5135,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="135.75" thickBot="1">
+    <row r="32" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A32" s="20">
         <v>102</v>
       </c>
@@ -5153,13 +5155,13 @@
         <v>45029</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H32" s="24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I32" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J32" s="33" t="s">
         <v>73</v>
@@ -5172,13 +5174,13 @@
         <v>73</v>
       </c>
       <c r="N32" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O32" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P32" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="26"/>
@@ -5187,7 +5189,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="135.75" thickBot="1">
+    <row r="33" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A33" s="20">
         <v>103</v>
       </c>
@@ -5207,13 +5209,13 @@
         <v>45029</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J33" s="33" t="s">
         <v>73</v>
@@ -5226,13 +5228,13 @@
         <v>73</v>
       </c>
       <c r="N33" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O33" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P33" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q33" s="25"/>
       <c r="R33" s="26"/>
@@ -5241,7 +5243,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="105.75" thickBot="1">
+    <row r="34" spans="1:20" ht="101.4" thickBot="1">
       <c r="A34" s="20">
         <v>104</v>
       </c>
@@ -5261,13 +5263,13 @@
         <v>45029</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H34" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I34" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>73</v>
@@ -5280,13 +5282,13 @@
         <v>73</v>
       </c>
       <c r="N34" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O34" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P34" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="26"/>
@@ -5295,7 +5297,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="135.75" thickBot="1">
+    <row r="35" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A35" s="20">
         <v>105</v>
       </c>
@@ -5333,7 +5335,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="135.75" thickBot="1">
+    <row r="36" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A36" s="20">
         <v>106</v>
       </c>
@@ -5353,13 +5355,13 @@
         <v>45029</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H36" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I36" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J36" s="33" t="s">
         <v>73</v>
@@ -5372,13 +5374,13 @@
         <v>73</v>
       </c>
       <c r="N36" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O36" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P36" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q36" s="25"/>
       <c r="R36" s="26"/>
@@ -5387,7 +5389,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="120.75" thickBot="1">
+    <row r="37" spans="1:20" ht="115.8" thickBot="1">
       <c r="A37" s="20">
         <v>107</v>
       </c>
@@ -5425,7 +5427,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="120.75" thickBot="1">
+    <row r="38" spans="1:20" ht="115.8" thickBot="1">
       <c r="A38" s="20">
         <v>108</v>
       </c>
@@ -5463,7 +5465,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="120.75" thickBot="1">
+    <row r="39" spans="1:20" ht="115.8" thickBot="1">
       <c r="A39" s="20">
         <v>109</v>
       </c>
@@ -5501,7 +5503,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="105.75" thickBot="1">
+    <row r="40" spans="1:20" ht="101.4" thickBot="1">
       <c r="A40" s="20">
         <v>110</v>
       </c>
@@ -5521,13 +5523,13 @@
         <v>45029</v>
       </c>
       <c r="G40" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H40" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I40" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J40" s="33" t="s">
         <v>73</v>
@@ -5540,13 +5542,13 @@
         <v>73</v>
       </c>
       <c r="N40" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O40" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P40" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q40" s="25"/>
       <c r="R40" s="26"/>
@@ -5555,7 +5557,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="120.75" thickBot="1">
+    <row r="41" spans="1:20" ht="115.8" thickBot="1">
       <c r="A41" s="20">
         <v>111</v>
       </c>
@@ -5593,7 +5595,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="120.75" thickBot="1">
+    <row r="42" spans="1:20" ht="115.8" thickBot="1">
       <c r="A42" s="20">
         <v>112</v>
       </c>
@@ -5631,7 +5633,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="120.75" thickBot="1">
+    <row r="43" spans="1:20" ht="115.8" thickBot="1">
       <c r="A43" s="20">
         <v>113</v>
       </c>
@@ -5669,7 +5671,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="120.75" thickBot="1">
+    <row r="44" spans="1:20" ht="115.8" thickBot="1">
       <c r="A44" s="20">
         <v>114</v>
       </c>
@@ -5689,13 +5691,13 @@
         <v>45029</v>
       </c>
       <c r="G44" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J44" s="33" t="s">
         <v>73</v>
@@ -5708,13 +5710,13 @@
         <v>73</v>
       </c>
       <c r="N44" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O44" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P44" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q44" s="25"/>
       <c r="R44" s="26"/>
@@ -5723,7 +5725,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="120.75" thickBot="1">
+    <row r="45" spans="1:20" ht="115.8" thickBot="1">
       <c r="A45" s="20">
         <v>115</v>
       </c>
@@ -5761,7 +5763,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="120.75" thickBot="1">
+    <row r="46" spans="1:20" ht="115.8" thickBot="1">
       <c r="A46" s="20">
         <v>116</v>
       </c>
@@ -5781,13 +5783,13 @@
         <v>45029</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H46" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I46" s="32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J46" s="33" t="s">
         <v>73</v>
@@ -5800,13 +5802,13 @@
         <v>73</v>
       </c>
       <c r="N46" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O46" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P46" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="26"/>
@@ -5815,7 +5817,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="120.75" thickBot="1">
+    <row r="47" spans="1:20" ht="115.8" thickBot="1">
       <c r="A47" s="20">
         <v>117</v>
       </c>
@@ -5835,13 +5837,13 @@
         <v>45029</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J47" s="33" t="s">
         <v>73</v>
@@ -5854,13 +5856,13 @@
         <v>73</v>
       </c>
       <c r="N47" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O47" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P47" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
@@ -5869,7 +5871,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="120.75" thickBot="1">
+    <row r="48" spans="1:20" ht="115.8" thickBot="1">
       <c r="A48" s="20">
         <v>118</v>
       </c>
@@ -5889,13 +5891,13 @@
         <v>45029</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H48" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I48" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J48" s="33" t="s">
         <v>73</v>
@@ -5908,13 +5910,13 @@
         <v>73</v>
       </c>
       <c r="N48" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O48" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P48" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q48" s="25"/>
       <c r="R48" s="26"/>
@@ -5923,7 +5925,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="120.75" thickBot="1">
+    <row r="49" spans="1:20" ht="115.8" thickBot="1">
       <c r="A49" s="20">
         <v>119</v>
       </c>
@@ -5961,7 +5963,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="120.75" thickBot="1">
+    <row r="50" spans="1:20" ht="115.8" thickBot="1">
       <c r="A50" s="20">
         <v>120</v>
       </c>
@@ -5981,13 +5983,13 @@
         <v>45035</v>
       </c>
       <c r="G50" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="H50" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="H50" s="24" t="s">
+      <c r="I50" s="24" t="s">
         <v>208</v>
-      </c>
-      <c r="I50" s="24" t="s">
-        <v>209</v>
       </c>
       <c r="J50" s="33" t="s">
         <v>73</v>
@@ -6000,13 +6002,13 @@
         <v>73</v>
       </c>
       <c r="N50" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O50" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P50" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q50" s="25"/>
       <c r="R50" s="26"/>
@@ -6015,7 +6017,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="120">
+    <row r="51" spans="1:20" ht="115.2">
       <c r="A51" s="20">
         <v>121</v>
       </c>
@@ -6035,13 +6037,13 @@
         <v>45037</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H51" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="I51" s="24" t="s">
         <v>219</v>
-      </c>
-      <c r="I51" s="24" t="s">
-        <v>220</v>
       </c>
       <c r="J51" s="33" t="s">
         <v>73</v>
@@ -6054,13 +6056,13 @@
         <v>73</v>
       </c>
       <c r="N51" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O51" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P51" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q51" s="25"/>
       <c r="R51" s="26"/>
@@ -15713,15 +15715,15 @@
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
     <col min="4" max="4" width="102" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="26" width="8.85546875" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1">
@@ -16725,11 +16727,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="26" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="26" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>